<commit_message>
Tests fixed and wondows support implemented for generating the reports
</commit_message>
<xml_diff>
--- a/AutomationFramework/params/SBI_params_test_ Almagro_Sept_2020_v1.xlsx
+++ b/AutomationFramework/params/SBI_params_test_ Almagro_Sept_2020_v1.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="272">
   <si>
     <t xml:space="preserve">TEST BLOCK</t>
   </si>
@@ -909,7 +909,13 @@
     <t xml:space="preserve">/routing-policy/policy-definitions/policy-definition/statements/statement/conditions/oc-bgp-pol:bgp-conditions/oc-bgp-pol:match-ext-community-set/oc-bgp-pol:config/oc-bgp-pol:ext-community-set</t>
   </si>
   <si>
-    <t xml:space="preserve">/routing-policy/policy-definitions/policy-definition/statements/statement/conditions/oc-bgp-pol:bgp-conditions/oc-bgp-pol:match-ext-community-set/oc-bgp-pol:config/oc-bgp-pol:match-set-options </t>
+    <t xml:space="preserve">oc-bgp-pol:match-set-options // oc-bgp-pol:ext-community-set </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rp_policy_def_match_set_options.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/routing-policy/policy-definitions/policy-definition/statements/statement/conditions/oc-bgp-pol:bgp-conditions/oc-bgp-pol:match-ext-community-set/oc-bgp-pol:config/oc-bgp-pol:match-set-options – /routing-policy/policy-definitions/policy-definition/statements/statement/conditions/oc-bgp-pol:bgp-conditions/oc-bgp-pol:match-ext-community-set/oc-bgp-pol:config/oc-bgp-pol:ext-community-set </t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -1337,8 +1343,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B45" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A135" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A151" activeCellId="0" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7447,37 +7453,35 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="7" t="s">
         <v>254</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C152" s="8" t="str">
-        <f aca="false">TRIM(RIGHT(SUBSTITUTE(G152,"/",REPT(" ","500")),500))</f>
-        <v>oc-bgp-pol:match-set-options</v>
+      <c r="C152" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="D152" s="8" t="str">
         <f aca="false">IFERROR(IF(SEARCH("state/",G152),"STATE","CONFIG"),"CONFIG")</f>
         <v>CONFIG</v>
       </c>
-      <c r="E152" s="8" t="str">
-        <f aca="false">SUBSTITUTE(CONCATENATE(A152,"_",B152,"_",IFERROR(MID(C152,FIND(":",C152)+1,LEN(C152)-FIND(":",C152)),C152),".","xml"),"-","_")</f>
-        <v>rp_policy_def_match_set_options.xml</v>
+      <c r="E152" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="F152" s="8" t="str">
         <f aca="false">CONCATENATE(A152,"_",B152,".yml")</f>
         <v>rp_policy_def.yml</v>
       </c>
-      <c r="G152" s="9" t="s">
-        <v>264</v>
+      <c r="G152" s="0" t="s">
+        <v>266</v>
       </c>
       <c r="H152" s="10" t="s">
         <v>257</v>
       </c>
       <c r="I152" s="13" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="J152" s="12" t="s">
         <v>16</v>
@@ -7520,13 +7524,13 @@
         <v>rp_policy_def.yml</v>
       </c>
       <c r="G153" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="H153" s="10" t="s">
         <v>257</v>
       </c>
       <c r="I153" s="11" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J153" s="12" t="s">
         <v>16</v>
@@ -7538,7 +7542,7 @@
         <v>17</v>
       </c>
       <c r="N153" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="O153" s="0" t="n">
         <f aca="false">COUNTIF($L$2:$L$153,N153)</f>
@@ -7546,15 +7550,15 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="G2:G153">
+  <conditionalFormatting sqref="G153 G2:G151">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -7665,7 +7669,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="26" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>